<commit_message>
Updated S–V curves & docs
</commit_message>
<xml_diff>
--- a/docs/Metrics for 2011 Plans.xlsx
+++ b/docs/Metrics for 2011 Plans.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alecramsay/Documents/Professional/Projects/Redistricting/DRA2020/analytics/partisan/experimental/3 - Analysis of 2011 Plans/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alecramsay/dev/bias-irl/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E3D30FD-C3D0-6E44-8FE0-D73FB4B27539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFBB9E57-2165-FE46-9F45-37CFFA8BDFEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1420" yWindow="500" windowWidth="27560" windowHeight="17500" activeTab="1" xr2:uid="{F08C87BC-C96D-1A4F-8DA4-EEEA4D15A1AA}"/>
+    <workbookView xWindow="1240" yWindow="500" windowWidth="27560" windowHeight="17500" activeTab="1" xr2:uid="{F08C87BC-C96D-1A4F-8DA4-EEEA4D15A1AA}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 3–2a" sheetId="1" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="72">
   <si>
     <t xml:space="preserve"> &lt;V&gt;</t>
   </si>
@@ -263,6 +263,30 @@
   </si>
   <si>
     <t>UR-2 -- [EG] | [gamma]</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>The unit of measure is a difference of seat shares.</t>
+  </si>
+  <si>
+    <t>Super-proportional outcomes can’t favor the minority party.</t>
+  </si>
+  <si>
+    <t>Sub-proportional outcomes favor the minority party.</t>
+  </si>
+  <si>
+    <t>Locality &lt;&lt;&lt; Proximate cause???</t>
   </si>
 </sst>
 </file>
@@ -273,7 +297,7 @@
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -309,8 +333,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="5" tint="0.39997558519241921"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -335,8 +366,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -430,11 +479,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -692,6 +756,45 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2650,13 +2753,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:V25"/>
+  <dimension ref="A1:V33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M6" sqref="M6"/>
+      <selection pane="bottomRight" activeCell="S28" sqref="S28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3693,31 +3796,31 @@
       </c>
       <c r="E14" s="22"/>
       <c r="F14" s="44"/>
-      <c r="G14" s="23" t="str">
+      <c r="G14" s="94" t="str">
         <f>G1</f>
         <v xml:space="preserve"> Decl</v>
       </c>
-      <c r="H14" s="27" t="str">
+      <c r="H14" s="95" t="str">
         <f>H1</f>
         <v xml:space="preserve"> LO</v>
       </c>
-      <c r="I14" s="25" t="str">
+      <c r="I14" s="96" t="str">
         <f>I1</f>
         <v xml:space="preserve"> MM</v>
       </c>
-      <c r="J14" s="23" t="str">
+      <c r="J14" s="98" t="str">
         <f>J1</f>
         <v xml:space="preserve"> BS_50</v>
       </c>
-      <c r="K14" s="24" t="str">
+      <c r="K14" s="97" t="str">
         <f t="shared" ref="K14:M14" si="0">K1</f>
         <v xml:space="preserve"> BV_50</v>
       </c>
-      <c r="L14" s="25" t="str">
+      <c r="L14" s="99" t="str">
         <f>L1</f>
         <v>β</v>
       </c>
-      <c r="M14" s="24" t="str">
+      <c r="M14" s="97" t="str">
         <f t="shared" si="0"/>
         <v xml:space="preserve"> GS</v>
       </c>
@@ -3742,7 +3845,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="30"/>
       <c r="D15" s="34" t="s">
         <v>15</v>
@@ -3788,7 +3891,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="30"/>
       <c r="D16" s="34" t="s">
         <v>17</v>
@@ -3805,7 +3908,7 @@
         <f t="shared" si="1"/>
         <v>*</v>
       </c>
-      <c r="J16" s="36" t="str">
+      <c r="J16" s="100" t="str">
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
@@ -3813,7 +3916,7 @@
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
-      <c r="L16" s="37" t="str">
+      <c r="L16" s="101" t="str">
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
@@ -3829,7 +3932,7 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="P16" s="37" t="str">
+      <c r="P16" s="102" t="str">
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
@@ -3860,7 +3963,7 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="L17" s="37" t="str">
+      <c r="L17" s="101" t="str">
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
@@ -3882,7 +3985,7 @@
       </c>
       <c r="V17"/>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="30"/>
       <c r="D18" s="34" t="s">
         <v>16</v>
@@ -3899,7 +4002,7 @@
         <f t="shared" si="1"/>
         <v>*</v>
       </c>
-      <c r="J18" s="36" t="str">
+      <c r="J18" s="100" t="str">
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
@@ -3929,7 +4032,7 @@
       </c>
       <c r="V18"/>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="30"/>
       <c r="D19" s="34" t="s">
         <v>19</v>
@@ -3946,7 +4049,7 @@
         <f t="shared" si="1"/>
         <v>*</v>
       </c>
-      <c r="J19" s="36" t="str">
+      <c r="J19" s="100" t="str">
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
@@ -3954,7 +4057,7 @@
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
-      <c r="L19" s="37" t="str">
+      <c r="L19" s="101" t="str">
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
@@ -3966,11 +4069,11 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="O19" s="37" t="str">
+      <c r="O19" s="102" t="str">
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
-      <c r="P19" s="37" t="str">
+      <c r="P19" s="102" t="str">
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
@@ -4139,7 +4242,7 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="L23" s="37" t="str">
+      <c r="L23" s="101" t="str">
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
@@ -4185,7 +4288,7 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="L24" s="37" t="str">
+      <c r="L24" s="101" t="str">
         <f t="shared" si="2"/>
         <v>X</v>
       </c>
@@ -4260,6 +4363,45 @@
       <c r="T25" s="69"/>
       <c r="U25" s="69"/>
       <c r="V25" s="7"/>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="K26" s="11"/>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="D30" s="90"/>
+      <c r="E30" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="G30" s="42" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="D31" s="92"/>
+      <c r="E31" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="G31" s="42" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="D32" s="91"/>
+      <c r="E32" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="G32" s="42" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D33" s="93"/>
+      <c r="E33" s="32" t="s">
+        <v>67</v>
+      </c>
+      <c r="G33" s="42" t="s">
+        <v>70</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>